<commit_message>
Update multiple Excel data files with new content
</commit_message>
<xml_diff>
--- a/Boletín 1/Data/Gini_ALC_tableau.xlsx
+++ b/Boletín 1/Data/Gini_ALC_tableau.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,62 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>pais</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Argentina</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Brasil</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Chile</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Colombia</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Paraguay</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Perú</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Uruguay</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Mexico</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>ALC</t>
+          <t>valor</t>
         </is>
       </c>
     </row>
@@ -504,142 +454,481 @@
       <c r="A2" t="n">
         <v>2005</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.6340000033378601</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>0.5519999861717224</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>0.550000011920929</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.5220000147819519</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.5239999890327454</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.5249999761581421</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="n">
-        <v>0.4760000109672546</v>
-      </c>
-      <c r="M2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ALC</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>0.5230000019073486</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2011</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.4709999859333038</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>0.5260000228881836</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.4760000109672546</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.5450000166893005</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.4580000042915344</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.5350000262260437</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.4629999995231628</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.4129999876022339</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.4839999973773956</v>
+        <v>2005</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.6340000033378601</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2015</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="n">
-        <v>0.5109999775886536</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.4620000123977661</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.5239999890327454</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.4620000123977661</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.4939999878406525</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.4490000009536743</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.3919999897480011</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="n">
-        <v>0.4959999918937683</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.4659999907016754</v>
+        <v>2005</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5519999861717224</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Colombia</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.550000011920929</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.4760000109672546</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5220000147819519</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Paraguay</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.5239999890327454</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.5249999761581421</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ALC</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.4839999973773956</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.4709999859333038</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.5260000228881836</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.4760000109672546</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Colombia</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.5450000166893005</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.4580000042915344</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Paraguay</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.5350000262260437</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.4629999995231628</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.4129999876022339</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ALC</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.4659999907016754</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.5109999775886536</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.4620000123977661</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Colombia</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.5239999890327454</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0.4959999918937683</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.4620000123977661</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Paraguay</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.4939999878406525</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.4490000009536743</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0.3919999897480011</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
         <v>2023</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ALC</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0.4519999921321869</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
         <v>0.4359999895095825</v>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="n">
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
         <v>0.5149999856948853</v>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Colombia</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
         <v>0.5600000023841858</v>
       </c>
-      <c r="G5" t="n">
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0.4799999892711639</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
         <v>0.4420000016689301</v>
       </c>
-      <c r="H5" t="n">
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Paraguay</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
         <v>0.4600000083446503</v>
       </c>
-      <c r="I5" t="n">
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
         <v>0.4169999957084656</v>
       </c>
-      <c r="J5" t="n">
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
         <v>0.4040000140666962</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
-        <v>0.4799999892711639</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.4519999921321869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>